<commit_message>
Some fix Print list tabs
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestExcelFile2.xlsx
+++ b/src/test/resources/data/TestExcelFile2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\G46Automation\src\test\resources\data\"/>
     </mc:Choice>
@@ -13,10 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="New Лист" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
   <si>
     <t>Test1</t>
   </si>
@@ -84,12 +85,28 @@
   </si>
   <si>
     <t>Test20</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,7 +422,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F15"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,4 +730,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>